<commit_message>
luu y sua file
</commit_message>
<xml_diff>
--- a/API Specs VY2-G06.xlsx
+++ b/API Specs VY2-G06.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SV\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HUFLIT\Nam 3 HK2\Công nghệ phần mềm nâng cao\VY2-G06-Tour-Traveloka-fe\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEDE9A4-11FA-4CCB-9AE5-F669D91CBF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -146,7 +147,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -503,26 +504,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -551,7 +552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -572,7 +573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -599,7 +600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -626,7 +627,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -653,7 +654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -680,7 +681,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -707,7 +708,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -734,7 +735,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -761,7 +762,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -774,7 +775,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -787,7 +788,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -800,7 +801,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -813,7 +814,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -826,7 +827,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -839,7 +840,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -852,7 +853,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
up laij db va file api
</commit_message>
<xml_diff>
--- a/API Specs VY2-G06.xlsx
+++ b/API Specs VY2-G06.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HUFLIT\Nam 3 HK2\Công nghệ phần mềm nâng cao\VY2-G06-Tour-Traveloka-fe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qtthi\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEDE9A4-11FA-4CCB-9AE5-F669D91CBF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090EE74C-A325-4B4E-BDC8-5178A2AF5F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="71">
   <si>
     <t>Tên App</t>
   </si>
@@ -87,9 +87,6 @@
     <t>GET</t>
   </si>
   <si>
-    <t>localhost:3000/api/getvoucher</t>
-  </si>
-  <si>
     <t>AppID, UserID,Voucher</t>
   </si>
   <si>
@@ -108,47 +105,152 @@
     <t>Get danh sách khung giá</t>
   </si>
   <si>
-    <t>localhost:3000/api/UsedVoucher</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
-    <t xml:space="preserve">Post danh sách voucher mà user đã sử dụng </t>
-  </si>
-  <si>
-    <t>localhost:3000/api/UsedGift</t>
-  </si>
-  <si>
     <t>AppID, UserID,Gift</t>
   </si>
   <si>
     <t xml:space="preserve">Post danh sách gift mà user đã sử dụng </t>
   </si>
   <si>
-    <t>localhost:3000/api/HistoryTransacsion</t>
-  </si>
-  <si>
-    <t>localhost:3000/api/khunggia</t>
-  </si>
-  <si>
-    <t>localhost:3000/api/getlistgift</t>
-  </si>
-  <si>
     <t>AppID, UserID,TranID, TourName, Price, SttBooking,Point</t>
   </si>
   <si>
     <t>Post idgiaodich, tentour, gia, trang thai giao dich để Vy1 lưu vào lịch sử giao dịch</t>
   </si>
   <si>
-    <t>localhost:3000/api/login</t>
+    <t>idactivity, id schedule, idpartner, country, city, type, name, place,price,amount,stt,timestart,endtime, desc</t>
+  </si>
+  <si>
+    <t>lây dữ liệu từ post và insert vào db</t>
+  </si>
+  <si>
+    <t>idbooking, idschedule, idcustomer, total, sttbooking, amountpeople, tourtimestart, phonemunber, reservationist, discount</t>
+  </si>
+  <si>
+    <t>get dữ liệu booking từ FE</t>
+  </si>
+  <si>
+    <t>get dữ liệu thanh toán</t>
+  </si>
+  <si>
+    <t>iduser, idsearch, keyword</t>
+  </si>
+  <si>
+    <t>idfavoutite, iduser, idactivyti</t>
+  </si>
+  <si>
+    <t>iduser, name, phone, email, address, gender</t>
+  </si>
+  <si>
+    <t>get dữ liệu của user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get dữ liệu yêu thích của user </t>
+  </si>
+  <si>
+    <t>idpartner, partnername</t>
+  </si>
+  <si>
+    <t>get dữ liệu của partner</t>
+  </si>
+  <si>
+    <t>UserLogin</t>
+  </si>
+  <si>
+    <t>GetVoucher</t>
+  </si>
+  <si>
+    <t>GetListGift</t>
+  </si>
+  <si>
+    <t>GetKhungGia</t>
+  </si>
+  <si>
+    <t>PostUseVoucher</t>
+  </si>
+  <si>
+    <t>PostUseGift</t>
+  </si>
+  <si>
+    <t>PostHtrTransacsion</t>
+  </si>
+  <si>
+    <t>PostDetailActivity</t>
+  </si>
+  <si>
+    <t>GetBookingActivity</t>
+  </si>
+  <si>
+    <t>GetKeySearch</t>
+  </si>
+  <si>
+    <t>GetFavourite</t>
+  </si>
+  <si>
+    <t>GetCustomer</t>
+  </si>
+  <si>
+    <t>PostPartner</t>
+  </si>
+  <si>
+    <t>PostDetailcustomer</t>
+  </si>
+  <si>
+    <t>PostKeysearch</t>
+  </si>
+  <si>
+    <t>PostFavourite</t>
+  </si>
+  <si>
+    <t>PostCountryActivity</t>
+  </si>
+  <si>
+    <t>PostCityActivity</t>
+  </si>
+  <si>
+    <t>PostFilterCountryActivity</t>
+  </si>
+  <si>
+    <t>PostFilterCityActivity</t>
+  </si>
+  <si>
+    <t>PostFilterActyvitySchedule</t>
+  </si>
+  <si>
+    <t>PostFilterActyvityImages</t>
+  </si>
+  <si>
+    <t>VY2-G01</t>
+  </si>
+  <si>
+    <t>VY2-G09</t>
+  </si>
+  <si>
+    <t>rest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xóa tour đặt </t>
+  </si>
+  <si>
+    <t>put activity</t>
+  </si>
+  <si>
+    <t>put</t>
+  </si>
+  <si>
+    <t>Post danh sách voucher mà user đã sử dụng (update voucher )</t>
+  </si>
+  <si>
+    <t>iduser, idfavourit, idactivity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,8 +266,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,8 +286,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -213,16 +327,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -505,19 +652,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.77734375" style="16" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
@@ -536,7 +683,7 @@
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -552,7 +699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -563,7 +710,7 @@
       <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="4"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1">
@@ -573,281 +720,397 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="4" t="s">
+    <row r="3" spans="1:9" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="1">
-        <v>200</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="H3" s="7">
+        <v>200</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="7">
+        <v>200</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="7">
+        <v>200</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
+      <c r="F6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="10">
+        <v>200</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="E7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1">
-        <v>200</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
+      <c r="G7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="10">
+        <v>200</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="10">
+        <v>200</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="10">
+        <v>200</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="1">
+        <v>200</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="E11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="1">
-        <v>200</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="1">
-        <v>200</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="1">
-        <v>200</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="1">
-        <v>200</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="1">
-        <v>200</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="H11" s="1">
+        <v>200</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="B12" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="1">
+        <v>200</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="B13" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="1">
+        <v>200</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="B14" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="1">
+        <v>200</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+      <c r="B15" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="1">
+        <v>200</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="B16" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="4"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -857,16 +1120,166 @@
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="B17" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="4"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
sua lại db và api
</commit_message>
<xml_diff>
--- a/API Specs VY2-G06.xlsx
+++ b/API Specs VY2-G06.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qtthi\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090EE74C-A325-4B4E-BDC8-5178A2AF5F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41187C5-B9E5-430D-905D-06E7CC437621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="82">
   <si>
     <t>Tên App</t>
   </si>
@@ -71,19 +71,9 @@
     <t>VY2-G06</t>
   </si>
   <si>
-    <t xml:space="preserve">POST
-</t>
-  </si>
-  <si>
     <t>JSON</t>
   </si>
   <si>
-    <t>AppID, UserID,Token</t>
-  </si>
-  <si>
-    <t>chuyển Token local storage</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
@@ -99,9 +89,6 @@
     <t>Get danh sách listgift</t>
   </si>
   <si>
-    <t>AppID, UserID,ListPrice</t>
-  </si>
-  <si>
     <t>Get danh sách khung giá</t>
   </si>
   <si>
@@ -111,12 +98,6 @@
     <t>AppID, UserID,Gift</t>
   </si>
   <si>
-    <t xml:space="preserve">Post danh sách gift mà user đã sử dụng </t>
-  </si>
-  <si>
-    <t>AppID, UserID,TranID, TourName, Price, SttBooking,Point</t>
-  </si>
-  <si>
     <t>Post idgiaodich, tentour, gia, trang thai giao dich để Vy1 lưu vào lịch sử giao dịch</t>
   </si>
   <si>
@@ -150,12 +131,6 @@
     <t xml:space="preserve">get dữ liệu yêu thích của user </t>
   </si>
   <si>
-    <t>idpartner, partnername</t>
-  </si>
-  <si>
-    <t>get dữ liệu của partner</t>
-  </si>
-  <si>
     <t>UserLogin</t>
   </si>
   <si>
@@ -165,18 +140,12 @@
     <t>GetListGift</t>
   </si>
   <si>
-    <t>GetKhungGia</t>
-  </si>
-  <si>
     <t>PostUseVoucher</t>
   </si>
   <si>
     <t>PostUseGift</t>
   </si>
   <si>
-    <t>PostHtrTransacsion</t>
-  </si>
-  <si>
     <t>PostDetailActivity</t>
   </si>
   <si>
@@ -192,9 +161,6 @@
     <t>GetCustomer</t>
   </si>
   <si>
-    <t>PostPartner</t>
-  </si>
-  <si>
     <t>PostDetailcustomer</t>
   </si>
   <si>
@@ -210,12 +176,6 @@
     <t>PostCityActivity</t>
   </si>
   <si>
-    <t>PostFilterCountryActivity</t>
-  </si>
-  <si>
-    <t>PostFilterCityActivity</t>
-  </si>
-  <si>
     <t>PostFilterActyvitySchedule</t>
   </si>
   <si>
@@ -231,19 +191,91 @@
     <t>rest</t>
   </si>
   <si>
-    <t xml:space="preserve">xóa tour đặt </t>
-  </si>
-  <si>
-    <t>put activity</t>
-  </si>
-  <si>
     <t>put</t>
   </si>
   <si>
-    <t>Post danh sách voucher mà user đã sử dụng (update voucher )</t>
-  </si>
-  <si>
     <t>iduser, idfavourit, idactivity</t>
+  </si>
+  <si>
+    <t>idcity, idcountry, cityname</t>
+  </si>
+  <si>
+    <t>idcountry, countryname, imageUrl</t>
+  </si>
+  <si>
+    <t>idschedul, idactivity, starttime, endtime</t>
+  </si>
+  <si>
+    <t>idimage, idactivity, link</t>
+  </si>
+  <si>
+    <t>idcustomer, name, phone, email,</t>
+  </si>
+  <si>
+    <t>gửi dữ liệu country cho FE</t>
+  </si>
+  <si>
+    <t>Gửi dữ liệu city cho FE</t>
+  </si>
+  <si>
+    <t>Gửi dữ liệu lịch trình tour cho FE</t>
+  </si>
+  <si>
+    <t>Gửi hình ảnh tour cho FE</t>
+  </si>
+  <si>
+    <t>Gửi thông tin khách hàng đã đăng nhập cho FE</t>
+  </si>
+  <si>
+    <t>Gửi từ khóa đã đăng nhập cho FE</t>
+  </si>
+  <si>
+    <t>Gửi dữ liệu yêu thích cho FE</t>
+  </si>
+  <si>
+    <t>PutActivity</t>
+  </si>
+  <si>
+    <t>idactivity, id schedule, idpartner, country, city, type, name, place,price,amount,stt, desc</t>
+  </si>
+  <si>
+    <t>gửi dữ liệu cho BE để chỉnh sửa activity</t>
+  </si>
+  <si>
+    <t>G06</t>
+  </si>
+  <si>
+    <t>postTourTransaction</t>
+  </si>
+  <si>
+    <t>AppID, UserID,TransactionID, ActivityName,StatusBooking, Voucher,Cost, Point</t>
+  </si>
+  <si>
+    <t>List String</t>
+  </si>
+  <si>
+    <t>AppID, UserID,LoginToken</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Lấy Token đăng nhập</t>
+  </si>
+  <si>
+    <t>getBaremServicePrice</t>
+  </si>
+  <si>
+    <t>AppID, ProductID, MinPrice, Max Price, Commission</t>
+  </si>
+  <si>
+    <t>List Object</t>
+  </si>
+  <si>
+    <t>Put voucher mà user đã sử dụng (update voucher )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Put gift mà user đã sử dụng </t>
   </si>
 </sst>
 </file>
@@ -293,7 +325,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -340,11 +372,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -353,7 +394,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -372,6 +412,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -664,7 +706,7 @@
     <col min="2" max="2" width="44.88671875" customWidth="1"/>
     <col min="3" max="3" width="25.21875" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.77734375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="59.77734375" style="15" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
@@ -683,7 +725,7 @@
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -720,230 +762,230 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="8" t="s">
+    <row r="3" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="6">
+        <v>200</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="6">
+        <v>200</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="6">
+        <v>200</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="9">
+        <v>200</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="7">
-        <v>200</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="E7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="F7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="9">
+        <v>200</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="9">
+        <v>200</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="9">
+        <v>200</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="7">
-        <v>200</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="F10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="7">
-        <v>200</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="10">
-        <v>200</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="10">
-        <v>200</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="10">
-        <v>200</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="10">
-        <v>200</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="H10" s="1">
         <v>200</v>
@@ -954,25 +996,25 @@
     </row>
     <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H11" s="1">
         <v>200</v>
@@ -983,25 +1025,25 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H12" s="1">
         <v>200</v>
@@ -1012,25 +1054,25 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H13" s="1">
         <v>200</v>
@@ -1041,25 +1083,25 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H14" s="1">
         <v>200</v>
@@ -1070,25 +1112,25 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="H15" s="1">
         <v>200</v>
@@ -1099,184 +1141,212 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" s="1">
+        <v>200</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="1">
+        <v>200</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="1">
+        <v>200</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H19" s="1">
+        <v>200</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
+      <c r="H20" s="1">
+        <v>200</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="1">
+        <v>201</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22" s="1">
+        <v>202</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="5" t="s">
-        <v>67</v>
-      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="F23" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>